<commit_message>
Update excel processor to handle sheet names and column processing
</commit_message>
<xml_diff>
--- a/checking_list.xlsx
+++ b/checking_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3384" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3260" uniqueCount="678">
   <si>
     <t>Item#</t>
   </si>
@@ -2432,18 +2432,6 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
@@ -4047,18 +4035,6 @@
       <c r="A97" t="s">
         <v>6</v>
       </c>
-      <c r="B97" t="s">
-        <v>6</v>
-      </c>
-      <c r="C97" t="s">
-        <v>6</v>
-      </c>
-      <c r="D97" t="s">
-        <v>6</v>
-      </c>
-      <c r="E97" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98">
@@ -5696,18 +5672,6 @@
       <c r="A194" t="s">
         <v>7</v>
       </c>
-      <c r="B194" t="s">
-        <v>7</v>
-      </c>
-      <c r="C194" t="s">
-        <v>7</v>
-      </c>
-      <c r="D194" t="s">
-        <v>7</v>
-      </c>
-      <c r="E194" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="195" spans="1:5">
       <c r="A195">
@@ -7141,18 +7105,6 @@
       <c r="A279" t="s">
         <v>8</v>
       </c>
-      <c r="B279" t="s">
-        <v>8</v>
-      </c>
-      <c r="C279" t="s">
-        <v>8</v>
-      </c>
-      <c r="D279" t="s">
-        <v>8</v>
-      </c>
-      <c r="E279" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="280" spans="1:5">
       <c r="A280">
@@ -8586,18 +8538,6 @@
       <c r="A364" t="s">
         <v>9</v>
       </c>
-      <c r="B364" t="s">
-        <v>9</v>
-      </c>
-      <c r="C364" t="s">
-        <v>9</v>
-      </c>
-      <c r="D364" t="s">
-        <v>9</v>
-      </c>
-      <c r="E364" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="365" spans="1:5">
       <c r="A365">
@@ -9487,18 +9427,6 @@
       <c r="A417" t="s">
         <v>10</v>
       </c>
-      <c r="B417" t="s">
-        <v>10</v>
-      </c>
-      <c r="C417" t="s">
-        <v>10</v>
-      </c>
-      <c r="D417" t="s">
-        <v>10</v>
-      </c>
-      <c r="E417" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="418" spans="1:5">
       <c r="A418">
@@ -10133,18 +10061,6 @@
       <c r="A455" t="s">
         <v>11</v>
       </c>
-      <c r="B455" t="s">
-        <v>11</v>
-      </c>
-      <c r="C455" t="s">
-        <v>11</v>
-      </c>
-      <c r="D455" t="s">
-        <v>11</v>
-      </c>
-      <c r="E455" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="456" spans="1:5">
       <c r="A456">
@@ -10728,18 +10644,6 @@
       <c r="A490" t="s">
         <v>12</v>
       </c>
-      <c r="B490" t="s">
-        <v>12</v>
-      </c>
-      <c r="C490" t="s">
-        <v>12</v>
-      </c>
-      <c r="D490" t="s">
-        <v>12</v>
-      </c>
-      <c r="E490" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="491" spans="1:5">
       <c r="A491">
@@ -11323,18 +11227,6 @@
       <c r="A525" t="s">
         <v>13</v>
       </c>
-      <c r="B525" t="s">
-        <v>13</v>
-      </c>
-      <c r="C525" t="s">
-        <v>13</v>
-      </c>
-      <c r="D525" t="s">
-        <v>13</v>
-      </c>
-      <c r="E525" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="526" spans="1:5">
       <c r="A526">
@@ -12513,18 +12405,6 @@
       <c r="A595" t="s">
         <v>14</v>
       </c>
-      <c r="B595" t="s">
-        <v>14</v>
-      </c>
-      <c r="C595" t="s">
-        <v>14</v>
-      </c>
-      <c r="D595" t="s">
-        <v>14</v>
-      </c>
-      <c r="E595" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="596" spans="1:5">
       <c r="A596">
@@ -13669,18 +13549,6 @@
       <c r="A663" t="s">
         <v>15</v>
       </c>
-      <c r="B663" t="s">
-        <v>15</v>
-      </c>
-      <c r="C663" t="s">
-        <v>15</v>
-      </c>
-      <c r="D663" t="s">
-        <v>15</v>
-      </c>
-      <c r="E663" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="664" spans="1:5">
       <c r="A664">
@@ -14808,18 +14676,6 @@
       <c r="A730" t="s">
         <v>16</v>
       </c>
-      <c r="B730" t="s">
-        <v>16</v>
-      </c>
-      <c r="C730" t="s">
-        <v>16</v>
-      </c>
-      <c r="D730" t="s">
-        <v>16</v>
-      </c>
-      <c r="E730" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="731" spans="1:5">
       <c r="A731">
@@ -15947,18 +15803,6 @@
       <c r="A797" t="s">
         <v>17</v>
       </c>
-      <c r="B797" t="s">
-        <v>17</v>
-      </c>
-      <c r="C797" t="s">
-        <v>17</v>
-      </c>
-      <c r="D797" t="s">
-        <v>17</v>
-      </c>
-      <c r="E797" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="798" spans="1:5">
       <c r="A798">
@@ -17103,18 +16947,6 @@
       <c r="A865" t="s">
         <v>18</v>
       </c>
-      <c r="B865" t="s">
-        <v>18</v>
-      </c>
-      <c r="C865" t="s">
-        <v>18</v>
-      </c>
-      <c r="D865" t="s">
-        <v>18</v>
-      </c>
-      <c r="E865" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="866" spans="1:5">
       <c r="A866">
@@ -18242,18 +18074,6 @@
       <c r="A932" t="s">
         <v>19</v>
       </c>
-      <c r="B932" t="s">
-        <v>19</v>
-      </c>
-      <c r="C932" t="s">
-        <v>19</v>
-      </c>
-      <c r="D932" t="s">
-        <v>19</v>
-      </c>
-      <c r="E932" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="933" spans="1:5">
       <c r="A933">
@@ -19109,18 +18929,6 @@
       <c r="A983" t="s">
         <v>20</v>
       </c>
-      <c r="B983" t="s">
-        <v>20</v>
-      </c>
-      <c r="C983" t="s">
-        <v>20</v>
-      </c>
-      <c r="D983" t="s">
-        <v>20</v>
-      </c>
-      <c r="E983" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="984" spans="1:5">
       <c r="A984">
@@ -19976,18 +19784,6 @@
       <c r="A1034" t="s">
         <v>21</v>
       </c>
-      <c r="B1034" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1034" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1034" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1034" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="1035" spans="1:5">
       <c r="A1035">
@@ -20843,18 +20639,6 @@
       <c r="A1085" t="s">
         <v>22</v>
       </c>
-      <c r="B1085" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1085" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1085" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1085" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="1086" spans="1:5">
       <c r="A1086">
@@ -21727,18 +21511,6 @@
       <c r="A1137" t="s">
         <v>23</v>
       </c>
-      <c r="B1137" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1137" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1137" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1137" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="1138" spans="1:5">
       <c r="A1138">
@@ -22594,18 +22366,6 @@
       <c r="A1188" t="s">
         <v>24</v>
       </c>
-      <c r="B1188" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1188" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1188" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1188" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="1189" spans="1:5">
       <c r="A1189">
@@ -23461,18 +23221,6 @@
       <c r="A1239" t="s">
         <v>25</v>
       </c>
-      <c r="B1239" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1239" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1239" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1239" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="1240" spans="1:5">
       <c r="A1240">
@@ -24328,18 +24076,6 @@
       <c r="A1290" t="s">
         <v>26</v>
       </c>
-      <c r="B1290" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1290" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1290" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1290" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="1291" spans="1:5">
       <c r="A1291">
@@ -25195,18 +24931,6 @@
       <c r="A1341" t="s">
         <v>27</v>
       </c>
-      <c r="B1341" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1341" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1341" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1341" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="1342" spans="1:5">
       <c r="A1342">
@@ -26062,18 +25786,6 @@
       <c r="A1392" t="s">
         <v>28</v>
       </c>
-      <c r="B1392" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1392" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1392" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1392" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="1393" spans="1:5">
       <c r="A1393">
@@ -27439,18 +27151,6 @@
       <c r="A1473" t="s">
         <v>29</v>
       </c>
-      <c r="B1473" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1473" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1473" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1473" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="1474" spans="1:5">
       <c r="A1474">
@@ -28816,18 +28516,6 @@
       <c r="A1554" t="s">
         <v>30</v>
       </c>
-      <c r="B1554" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1554" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1554" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1554" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="1555" spans="1:5">
       <c r="A1555">
@@ -30193,18 +29881,6 @@
       <c r="A1635" t="s">
         <v>31</v>
       </c>
-      <c r="B1635" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1635" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1635" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1635" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="1636" spans="1:5">
       <c r="A1636">
@@ -30227,18 +29903,6 @@
       <c r="A1637" t="s">
         <v>32</v>
       </c>
-      <c r="B1637" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1637" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1637" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1637" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="1638" spans="1:5">
       <c r="A1638">
@@ -30261,18 +29925,6 @@
       <c r="A1639" t="s">
         <v>33</v>
       </c>
-      <c r="B1639" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1639" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1639" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1639" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="1640" spans="1:5">
       <c r="A1640">
@@ -30295,18 +29947,6 @@
       <c r="A1641" t="s">
         <v>34</v>
       </c>
-      <c r="B1641" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1641" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1641" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1641" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="1642" spans="1:5">
       <c r="A1642">
@@ -30327,18 +29967,6 @@
     </row>
     <row r="1643" spans="1:5">
       <c r="A1643" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1643" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1643" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1643" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1643" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>